<commit_message>
make it easy to update sheets
</commit_message>
<xml_diff>
--- a/Excel/Test.xlsx
+++ b/Excel/Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="31785" yWindow="2325" windowWidth="21600" windowHeight="11505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="780" yWindow="2340" windowWidth="21600" windowHeight="11505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ScoutingInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -287,8 +287,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Y1000" headerRowCount="1" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A1:Y1000"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Y999" headerRowCount="1" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="A1:Y999"/>
   <tableColumns count="25">
     <tableColumn id="1" name="initials"/>
     <tableColumn id="2" name="event"/>
@@ -587,10 +587,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB399"/>
+  <dimension ref="A1:AB398"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="A2:Y1000"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -32479,7 +32479,7 @@
       <c r="R342" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="S342" t="inlineStr">
+      <c r="S342" s="14" t="inlineStr">
         <is>
           <t>x</t>
         </is>
@@ -32601,10 +32601,8 @@
       <c r="K344" s="14" t="n"/>
       <c r="L344" s="14" t="n"/>
       <c r="M344" s="14" t="n"/>
-      <c r="O344" s="14" t="n"/>
       <c r="Q344" s="14" t="n"/>
       <c r="R344" s="14" t="n"/>
-      <c r="S344" s="14" t="n"/>
       <c r="T344" s="14" t="n"/>
       <c r="U344" s="14" t="n"/>
       <c r="V344" s="14" t="n"/>
@@ -32637,8 +32635,10 @@
       <c r="K346" s="14" t="n"/>
       <c r="L346" s="14" t="n"/>
       <c r="M346" s="14" t="n"/>
+      <c r="O346" s="14" t="n"/>
       <c r="Q346" s="14" t="n"/>
       <c r="R346" s="14" t="n"/>
+      <c r="S346" s="14" t="n"/>
       <c r="T346" s="14" t="n"/>
       <c r="U346" s="14" t="n"/>
       <c r="V346" s="14" t="n"/>
@@ -32695,7 +32695,6 @@
       <c r="O349" s="14" t="n"/>
       <c r="Q349" s="14" t="n"/>
       <c r="R349" s="14" t="n"/>
-      <c r="S349" s="14" t="n"/>
       <c r="T349" s="14" t="n"/>
       <c r="U349" s="14" t="n"/>
       <c r="V349" s="14" t="n"/>
@@ -32711,7 +32710,6 @@
       <c r="K350" s="14" t="n"/>
       <c r="L350" s="14" t="n"/>
       <c r="M350" s="14" t="n"/>
-      <c r="O350" s="14" t="n"/>
       <c r="Q350" s="14" t="n"/>
       <c r="R350" s="14" t="n"/>
       <c r="T350" s="14" t="n"/>
@@ -32729,6 +32727,7 @@
       <c r="K351" s="14" t="n"/>
       <c r="L351" s="14" t="n"/>
       <c r="M351" s="14" t="n"/>
+      <c r="O351" s="14" t="n"/>
       <c r="Q351" s="14" t="n"/>
       <c r="R351" s="14" t="n"/>
       <c r="T351" s="14" t="n"/>
@@ -32749,6 +32748,7 @@
       <c r="O352" s="14" t="n"/>
       <c r="Q352" s="14" t="n"/>
       <c r="R352" s="14" t="n"/>
+      <c r="S352" s="14" t="n"/>
       <c r="T352" s="14" t="n"/>
       <c r="U352" s="14" t="n"/>
       <c r="V352" s="14" t="n"/>
@@ -32766,7 +32766,6 @@
       <c r="M353" s="14" t="n"/>
       <c r="O353" s="14" t="n"/>
       <c r="Q353" s="14" t="n"/>
-      <c r="R353" s="14" t="n"/>
       <c r="S353" s="14" t="n"/>
       <c r="T353" s="14" t="n"/>
       <c r="U353" s="14" t="n"/>
@@ -32785,7 +32784,6 @@
       <c r="M354" s="14" t="n"/>
       <c r="O354" s="14" t="n"/>
       <c r="Q354" s="14" t="n"/>
-      <c r="S354" s="14" t="n"/>
       <c r="T354" s="14" t="n"/>
       <c r="U354" s="14" t="n"/>
       <c r="V354" s="14" t="n"/>
@@ -32803,6 +32801,8 @@
       <c r="M355" s="14" t="n"/>
       <c r="O355" s="14" t="n"/>
       <c r="Q355" s="14" t="n"/>
+      <c r="R355" s="14" t="n"/>
+      <c r="S355" s="14" t="n"/>
       <c r="T355" s="14" t="n"/>
       <c r="U355" s="14" t="n"/>
       <c r="V355" s="14" t="n"/>
@@ -32840,7 +32840,6 @@
       <c r="O357" s="14" t="n"/>
       <c r="Q357" s="14" t="n"/>
       <c r="R357" s="14" t="n"/>
-      <c r="S357" s="14" t="n"/>
       <c r="T357" s="14" t="n"/>
       <c r="U357" s="14" t="n"/>
       <c r="V357" s="14" t="n"/>
@@ -32874,9 +32873,9 @@
       <c r="K359" s="14" t="n"/>
       <c r="L359" s="14" t="n"/>
       <c r="M359" s="14" t="n"/>
-      <c r="O359" s="14" t="n"/>
       <c r="Q359" s="14" t="n"/>
       <c r="R359" s="14" t="n"/>
+      <c r="S359" s="14" t="n"/>
       <c r="T359" s="14" t="n"/>
       <c r="U359" s="14" t="n"/>
       <c r="V359" s="14" t="n"/>
@@ -32912,7 +32911,6 @@
       <c r="M361" s="14" t="n"/>
       <c r="Q361" s="14" t="n"/>
       <c r="R361" s="14" t="n"/>
-      <c r="S361" s="14" t="n"/>
       <c r="T361" s="14" t="n"/>
       <c r="U361" s="14" t="n"/>
       <c r="V361" s="14" t="n"/>
@@ -32928,8 +32926,10 @@
       <c r="K362" s="14" t="n"/>
       <c r="L362" s="14" t="n"/>
       <c r="M362" s="14" t="n"/>
+      <c r="O362" s="14" t="n"/>
       <c r="Q362" s="14" t="n"/>
       <c r="R362" s="14" t="n"/>
+      <c r="S362" s="14" t="n"/>
       <c r="T362" s="14" t="n"/>
       <c r="U362" s="14" t="n"/>
       <c r="V362" s="14" t="n"/>
@@ -33002,7 +33002,6 @@
       <c r="K366" s="14" t="n"/>
       <c r="L366" s="14" t="n"/>
       <c r="M366" s="14" t="n"/>
-      <c r="O366" s="14" t="n"/>
       <c r="Q366" s="14" t="n"/>
       <c r="R366" s="14" t="n"/>
       <c r="S366" s="14" t="n"/>
@@ -33021,9 +33020,9 @@
       <c r="K367" s="14" t="n"/>
       <c r="L367" s="14" t="n"/>
       <c r="M367" s="14" t="n"/>
+      <c r="O367" s="14" t="n"/>
       <c r="Q367" s="14" t="n"/>
       <c r="R367" s="14" t="n"/>
-      <c r="S367" s="14" t="n"/>
       <c r="T367" s="14" t="n"/>
       <c r="U367" s="14" t="n"/>
       <c r="V367" s="14" t="n"/>
@@ -33078,6 +33077,7 @@
       <c r="O370" s="14" t="n"/>
       <c r="Q370" s="14" t="n"/>
       <c r="R370" s="14" t="n"/>
+      <c r="S370" s="14" t="n"/>
       <c r="T370" s="14" t="n"/>
       <c r="U370" s="14" t="n"/>
       <c r="V370" s="14" t="n"/>
@@ -33093,7 +33093,6 @@
       <c r="K371" s="14" t="n"/>
       <c r="L371" s="14" t="n"/>
       <c r="M371" s="14" t="n"/>
-      <c r="O371" s="14" t="n"/>
       <c r="Q371" s="14" t="n"/>
       <c r="R371" s="14" t="n"/>
       <c r="S371" s="14" t="n"/>
@@ -33112,6 +33111,7 @@
       <c r="K372" s="14" t="n"/>
       <c r="L372" s="14" t="n"/>
       <c r="M372" s="14" t="n"/>
+      <c r="O372" s="14" t="n"/>
       <c r="Q372" s="14" t="n"/>
       <c r="R372" s="14" t="n"/>
       <c r="S372" s="14" t="n"/>
@@ -33190,7 +33190,6 @@
       <c r="O376" s="14" t="n"/>
       <c r="Q376" s="14" t="n"/>
       <c r="R376" s="14" t="n"/>
-      <c r="S376" s="14" t="n"/>
       <c r="T376" s="14" t="n"/>
       <c r="U376" s="14" t="n"/>
       <c r="V376" s="14" t="n"/>
@@ -33263,6 +33262,7 @@
       <c r="O380" s="14" t="n"/>
       <c r="Q380" s="14" t="n"/>
       <c r="R380" s="14" t="n"/>
+      <c r="S380" s="14" t="n"/>
       <c r="T380" s="14" t="n"/>
       <c r="U380" s="14" t="n"/>
       <c r="V380" s="14" t="n"/>
@@ -33300,7 +33300,6 @@
       <c r="O382" s="14" t="n"/>
       <c r="Q382" s="14" t="n"/>
       <c r="R382" s="14" t="n"/>
-      <c r="S382" s="14" t="n"/>
       <c r="T382" s="14" t="n"/>
       <c r="U382" s="14" t="n"/>
       <c r="V382" s="14" t="n"/>
@@ -33373,6 +33372,7 @@
       <c r="O386" s="14" t="n"/>
       <c r="Q386" s="14" t="n"/>
       <c r="R386" s="14" t="n"/>
+      <c r="S386" s="14" t="n"/>
       <c r="T386" s="14" t="n"/>
       <c r="U386" s="14" t="n"/>
       <c r="V386" s="14" t="n"/>
@@ -33410,7 +33410,6 @@
       <c r="O388" s="14" t="n"/>
       <c r="Q388" s="14" t="n"/>
       <c r="R388" s="14" t="n"/>
-      <c r="S388" s="14" t="n"/>
       <c r="T388" s="14" t="n"/>
       <c r="U388" s="14" t="n"/>
       <c r="V388" s="14" t="n"/>
@@ -33426,7 +33425,6 @@
       <c r="K389" s="14" t="n"/>
       <c r="L389" s="14" t="n"/>
       <c r="M389" s="14" t="n"/>
-      <c r="O389" s="14" t="n"/>
       <c r="Q389" s="14" t="n"/>
       <c r="R389" s="14" t="n"/>
       <c r="T389" s="14" t="n"/>
@@ -33444,6 +33442,7 @@
       <c r="K390" s="14" t="n"/>
       <c r="L390" s="14" t="n"/>
       <c r="M390" s="14" t="n"/>
+      <c r="O390" s="14" t="n"/>
       <c r="Q390" s="14" t="n"/>
       <c r="R390" s="14" t="n"/>
       <c r="T390" s="14" t="n"/>
@@ -33515,7 +33514,6 @@
       <c r="K394" s="14" t="n"/>
       <c r="L394" s="14" t="n"/>
       <c r="M394" s="14" t="n"/>
-      <c r="O394" s="14" t="n"/>
       <c r="Q394" s="14" t="n"/>
       <c r="R394" s="14" t="n"/>
       <c r="T394" s="14" t="n"/>
@@ -33567,6 +33565,7 @@
       <c r="K397" s="14" t="n"/>
       <c r="L397" s="14" t="n"/>
       <c r="M397" s="14" t="n"/>
+      <c r="O397" s="14" t="n"/>
       <c r="Q397" s="14" t="n"/>
       <c r="R397" s="14" t="n"/>
       <c r="T397" s="14" t="n"/>
@@ -33593,24 +33592,6 @@
       <c r="W398" s="14" t="n"/>
       <c r="X398" s="14" t="n"/>
     </row>
-    <row r="399">
-      <c r="D399" s="14" t="n"/>
-      <c r="F399" s="14" t="n"/>
-      <c r="H399" s="14" t="n"/>
-      <c r="I399" s="14" t="n"/>
-      <c r="J399" s="14" t="n"/>
-      <c r="K399" s="14" t="n"/>
-      <c r="L399" s="14" t="n"/>
-      <c r="M399" s="14" t="n"/>
-      <c r="O399" s="14" t="n"/>
-      <c r="Q399" s="14" t="n"/>
-      <c r="R399" s="14" t="n"/>
-      <c r="T399" s="14" t="n"/>
-      <c r="U399" s="14" t="n"/>
-      <c r="V399" s="14" t="n"/>
-      <c r="W399" s="14" t="n"/>
-      <c r="X399" s="14" t="n"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>